<commit_message>
fixed t0 start, tau plts, err bars for rheology
</commit_message>
<xml_diff>
--- a/ariell_smith-rheology_hydrogels/2021-08-06-Hydrogels_AriellSmith_updated.xlsx
+++ b/ariell_smith-rheology_hydrogels/2021-08-06-Hydrogels_AriellSmith_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariel\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC5D6945-DABC-4CA2-B2C4-46484951B4C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B07C70-D522-4834-A6E9-8D89D7D50416}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="597" xr2:uid="{3E16EA9E-EC9A-45C8-B18C-C28CBCE15768}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="119">
   <si>
     <t>Shear Strain_ASCc5.5 [%]</t>
   </si>
@@ -369,6 +369,30 @@
   <si>
     <t>AriellSmith_ASC+Card_test2_05.06.2022_pH6.88_Sampleall_Lossmodulus_Average</t>
   </si>
+  <si>
+    <t>Standard deviation of Storage modulus_ test1_ASCc+Card</t>
+  </si>
+  <si>
+    <t>Standard deviation of Storage modulus_ASC+Card_test2</t>
+  </si>
+  <si>
+    <t>Standard deviation of Loss modulus_ASC+Card_test2</t>
+  </si>
+  <si>
+    <t>standard deviation of Loss modulus_ test1_ASCc+Card</t>
+  </si>
+  <si>
+    <t>Standard deviation _Storage modulus_ASC_test2</t>
+  </si>
+  <si>
+    <t>Standard deviation_Loss Modulus_ASC_test2</t>
+  </si>
+  <si>
+    <t>Standard deviation_Loss modulus_ASC_test1</t>
+  </si>
+  <si>
+    <t>Standard deviation_Storage modulus_ASC_test1</t>
+  </si>
 </sst>
 </file>
 
@@ -396,7 +420,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -415,6 +439,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -428,7 +458,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -437,6 +467,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -751,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A872D3A-BB0B-48E5-A0F0-DB242BA1B238}">
-  <dimension ref="A1:ES2974"/>
+  <dimension ref="A1:EZ2974"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AS1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="CL22" sqref="CL22"/>
+    <sheetView tabSelected="1" topLeftCell="DW1" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="EZ2" sqref="EZ2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -765,9 +797,10 @@
     <col min="24" max="24" width="8.7265625" style="4"/>
     <col min="52" max="52" width="9.1796875" style="4"/>
     <col min="101" max="101" width="8.7265625" style="4"/>
+    <col min="134" max="156" width="8.7265625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:148" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1065,44 +1098,68 @@
       <c r="EB1" t="s">
         <v>85</v>
       </c>
-      <c r="ED1" t="s">
+      <c r="ED1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="EE1" t="s">
+      <c r="EE1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="EF1" t="s">
+      <c r="EF1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="EH1" t="s">
+      <c r="EG1" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="EH1" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="EJ1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="EI1" t="s">
+      <c r="EK1" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="EJ1" t="s">
+      <c r="EL1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="EL1" t="s">
+      <c r="EM1" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="EN1" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="EP1" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="EM1" t="s">
+      <c r="EQ1" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="EN1" t="s">
+      <c r="ER1" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="EP1" t="s">
+      <c r="ES1" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="ET1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="EV1" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="EW1" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="EX1" s="8" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="2" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY1" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="EZ1" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>4.0399999999999998E-2</v>
       </c>
@@ -1421,54 +1478,86 @@
       <c r="EB2">
         <v>5.0815999999999999</v>
       </c>
-      <c r="ED2" s="2">
+      <c r="ED2" s="9">
         <v>0.1</v>
       </c>
-      <c r="EE2">
+      <c r="EE2" s="8">
         <f>AVERAGE(DO2,DW2)</f>
         <v>38.469000000000001</v>
       </c>
-      <c r="EF2">
+      <c r="EF2" s="8">
         <f>AVERAGE(DP2,DX2)</f>
         <v>4.0350999999999999</v>
       </c>
-      <c r="EH2" s="2">
+      <c r="EG2" s="8">
+        <f>STDEVA(DO2,DW2)</f>
+        <v>8.447097608054527</v>
+      </c>
+      <c r="EH2" s="8">
+        <f>STDEVA(DP2,DX2)</f>
+        <v>0.75009887348269499</v>
+      </c>
+      <c r="EJ2" s="9">
         <f>0.000992*100</f>
         <v>9.920000000000001E-2</v>
       </c>
-      <c r="EI2">
+      <c r="EK2" s="8">
         <f>AVERAGE(DS2,EA2)</f>
         <v>28.571000000000002</v>
       </c>
-      <c r="EJ2">
+      <c r="EL2" s="8">
         <f>AVERAGE(DT2,EB2)</f>
         <v>4.3147000000000002</v>
       </c>
-      <c r="EL2" s="2">
+      <c r="EM2" s="8">
+        <f>STDEVA(DS2,EA2)</f>
+        <v>7.3963369312112839</v>
+      </c>
+      <c r="EN2" s="8">
+        <f>STDEVA(DT2,EB2)</f>
+        <v>1.0845603809839284</v>
+      </c>
+      <c r="EP2" s="9">
         <v>0.1</v>
       </c>
-      <c r="EM2">
+      <c r="EQ2" s="8">
         <f>AVERAGE(CY2,DG2)</f>
         <v>157.91</v>
       </c>
-      <c r="EN2">
+      <c r="ER2" s="8">
         <f>AVERAGE(CZ2,DH2)</f>
         <v>31.981500000000004</v>
       </c>
-      <c r="EP2" s="2">
+      <c r="ES2" s="8">
+        <f>STDEVA(CY2,DG2)</f>
+        <v>52.057201230953623</v>
+      </c>
+      <c r="ET2" s="8">
+        <f>STDEVA(CZ2,DH2)</f>
+        <v>11.178651103778121</v>
+      </c>
+      <c r="EV2" s="9">
         <f>0.000992*100</f>
         <v>9.920000000000001E-2</v>
       </c>
-      <c r="EQ2">
+      <c r="EW2" s="8">
         <f>AVERAGE(DC2,DK2)</f>
         <v>206.86500000000001</v>
       </c>
-      <c r="ER2">
+      <c r="EX2" s="8">
         <f>AVERAGE(DD2,DL2)</f>
         <v>36.429499999999997</v>
       </c>
-    </row>
-    <row r="3" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY2" s="8">
+        <f>STDEVA(DC2,DK2)</f>
+        <v>91.379409332737552</v>
+      </c>
+      <c r="EZ2" s="8">
+        <f>STDEVA(DD2,DL2)</f>
+        <v>11.404925273757842</v>
+      </c>
+    </row>
+    <row r="3" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>4.19E-2</v>
       </c>
@@ -1787,54 +1876,86 @@
       <c r="EB3">
         <v>5.0533000000000001</v>
       </c>
-      <c r="ED3" s="2">
+      <c r="ED3" s="9">
         <v>0.13700000000000001</v>
       </c>
-      <c r="EE3">
+      <c r="EE3" s="8">
         <f>AVERAGE(DO3,DW3)</f>
         <v>40.664999999999999</v>
       </c>
-      <c r="EF3">
+      <c r="EF3" s="8">
         <f t="shared" ref="EF3:EF26" si="8">AVERAGE(DP3,DX3)</f>
         <v>3.9036499999999998</v>
       </c>
-      <c r="EH3" s="2">
+      <c r="EG3" s="8">
+        <f t="shared" ref="EG3:EG25" si="9">STDEVA(DO3,DW3)</f>
+        <v>8.8897464530772705</v>
+      </c>
+      <c r="EH3" s="8">
+        <f t="shared" ref="EH3:EH26" si="10">STDEVA(DP3,DX3)</f>
+        <v>0.61666782387278873</v>
+      </c>
+      <c r="EJ3" s="9">
         <f>0.00126*100</f>
         <v>0.126</v>
       </c>
-      <c r="EI3">
-        <f t="shared" ref="EI3:EI32" si="9">AVERAGE(DS3,EA3)</f>
+      <c r="EK3" s="8">
+        <f t="shared" ref="EK3:EK32" si="11">AVERAGE(DS3,EA3)</f>
         <v>28.932499999999997</v>
       </c>
-      <c r="EJ3">
-        <f t="shared" ref="EJ3:EJ32" si="10">AVERAGE(DT3,EB3)</f>
+      <c r="EL3" s="8">
+        <f t="shared" ref="EL3:EL32" si="12">AVERAGE(DT3,EB3)</f>
         <v>4.3072499999999998</v>
       </c>
-      <c r="EL3" s="2">
+      <c r="EM3" s="8">
+        <f t="shared" ref="EM3:EM32" si="13">STDEVA(DS3,EA3)</f>
+        <v>7.425328309239938</v>
+      </c>
+      <c r="EN3" s="8">
+        <f t="shared" ref="EN3:EN32" si="14">STDEVA(DT3,EB3)</f>
+        <v>1.0550740282084492</v>
+      </c>
+      <c r="EP3" s="9">
         <v>0.13700000000000001</v>
       </c>
-      <c r="EM3">
-        <f t="shared" ref="EM3:EM26" si="11">AVERAGE(CY3,DG3)</f>
+      <c r="EQ3" s="8">
+        <f t="shared" ref="EQ3:EQ26" si="15">AVERAGE(CY3,DG3)</f>
         <v>169.64</v>
       </c>
-      <c r="EN3">
-        <f t="shared" ref="EN3:EN26" si="12">AVERAGE(CZ3,DH3)</f>
+      <c r="ER3" s="8">
+        <f t="shared" ref="ER3:ER26" si="16">AVERAGE(CZ3,DH3)</f>
         <v>30.886000000000003</v>
       </c>
-      <c r="EP3" s="2">
+      <c r="ES3" s="8">
+        <f t="shared" ref="ES3:ES26" si="17">STDEVA(CY3,DG3)</f>
+        <v>53.697688963306561</v>
+      </c>
+      <c r="ET3" s="8">
+        <f t="shared" ref="ET3:ET26" si="18">STDEVA(CZ3,DH3)</f>
+        <v>9.9956614588530286</v>
+      </c>
+      <c r="EV3" s="9">
         <f>0.00126*100</f>
         <v>0.126</v>
       </c>
-      <c r="EQ3">
-        <f t="shared" ref="EQ3:EQ32" si="13">AVERAGE(DC3,DK3)</f>
+      <c r="EW3" s="8">
+        <f t="shared" ref="EW3:EW32" si="19">AVERAGE(DC3,DK3)</f>
         <v>210.17499999999998</v>
       </c>
-      <c r="ER3">
-        <f t="shared" ref="ER3:ER32" si="14">AVERAGE(DD3,DL3)</f>
+      <c r="EX3" s="8">
+        <f t="shared" ref="EX3:EX32" si="20">AVERAGE(DD3,DL3)</f>
         <v>36.726999999999997</v>
       </c>
-    </row>
-    <row r="4" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY3" s="8">
+        <f t="shared" ref="EY3:EY32" si="21">STDEVA(DC3,DK3)</f>
+        <v>90.47431265281871</v>
+      </c>
+      <c r="EZ3" s="8">
+        <f t="shared" ref="EZ3:EZ32" si="22">STDEVA(DD3,DL3)</f>
+        <v>11.339164343107486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>4.4999999999999998E-2</v>
       </c>
@@ -2153,54 +2274,86 @@
       <c r="EB4">
         <v>5.0740999999999996</v>
       </c>
-      <c r="ED4" s="2">
+      <c r="ED4" s="9">
         <v>0.188</v>
       </c>
-      <c r="EE4">
-        <f t="shared" ref="EE4:EE26" si="15">AVERAGE(DO4,DW4)</f>
+      <c r="EE4" s="8">
+        <f t="shared" ref="EE4:EE26" si="23">AVERAGE(DO4,DW4)</f>
         <v>42.278500000000001</v>
       </c>
-      <c r="EF4">
+      <c r="EF4" s="8">
         <f t="shared" si="8"/>
         <v>3.8616999999999999</v>
       </c>
-      <c r="EH4" s="2">
+      <c r="EG4" s="8">
+        <f t="shared" si="9"/>
+        <v>9.2468353775764918</v>
+      </c>
+      <c r="EH4" s="8">
+        <f t="shared" si="10"/>
+        <v>0.52269333265309581</v>
+      </c>
+      <c r="EJ4" s="9">
         <f>0.00158*100</f>
         <v>0.158</v>
       </c>
-      <c r="EI4">
-        <f t="shared" si="9"/>
+      <c r="EK4" s="8">
+        <f t="shared" si="11"/>
         <v>29.195500000000003</v>
       </c>
-      <c r="EJ4">
+      <c r="EL4" s="8">
         <f>AVERAGE(DT4,EB4)</f>
         <v>4.3453499999999998</v>
       </c>
-      <c r="EL4" s="2">
+      <c r="EM4" s="8">
+        <f t="shared" si="13"/>
+        <v>7.457855221174496</v>
+      </c>
+      <c r="EN4" s="8">
+        <f t="shared" si="14"/>
+        <v>1.030608133579394</v>
+      </c>
+      <c r="EP4" s="9">
         <v>0.188</v>
       </c>
-      <c r="EM4">
-        <f t="shared" si="11"/>
+      <c r="EQ4" s="8">
+        <f t="shared" si="15"/>
         <v>178.70500000000001</v>
       </c>
-      <c r="EN4">
-        <f t="shared" si="12"/>
+      <c r="ER4" s="8">
+        <f t="shared" si="16"/>
         <v>30.183999999999997</v>
       </c>
-      <c r="EP4" s="2">
+      <c r="ES4" s="8">
+        <f t="shared" si="17"/>
+        <v>54.977552237254137</v>
+      </c>
+      <c r="ET4" s="8">
+        <f t="shared" si="18"/>
+        <v>9.239057202983437</v>
+      </c>
+      <c r="EV4" s="9">
         <f>0.00158*100</f>
         <v>0.158</v>
       </c>
-      <c r="EQ4">
-        <f t="shared" si="13"/>
+      <c r="EW4" s="8">
+        <f t="shared" si="19"/>
         <v>212.565</v>
       </c>
-      <c r="ER4">
-        <f t="shared" si="14"/>
+      <c r="EX4" s="8">
+        <f t="shared" si="20"/>
         <v>36.755499999999998</v>
       </c>
-    </row>
-    <row r="5" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY4" s="8">
+        <f t="shared" si="21"/>
+        <v>89.470221023533881</v>
+      </c>
+      <c r="EZ4" s="8">
+        <f t="shared" si="22"/>
+        <v>11.130567842657458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>5.8299999999999998E-2</v>
       </c>
@@ -2519,54 +2672,86 @@
       <c r="EB5">
         <v>5.0837000000000003</v>
       </c>
-      <c r="ED5" s="2">
+      <c r="ED5" s="9">
         <v>0.25900000000000001</v>
       </c>
-      <c r="EE5">
-        <f t="shared" si="15"/>
+      <c r="EE5" s="8">
+        <f t="shared" si="23"/>
         <v>43.593999999999994</v>
       </c>
-      <c r="EF5">
+      <c r="EF5" s="8">
         <f t="shared" si="8"/>
         <v>3.8675499999999996</v>
       </c>
-      <c r="EH5" s="2">
+      <c r="EG5" s="8">
+        <f t="shared" si="9"/>
+        <v>9.4271476067790907</v>
+      </c>
+      <c r="EH5" s="8">
+        <f t="shared" si="10"/>
+        <v>0.44950778080028786</v>
+      </c>
+      <c r="EJ5" s="9">
         <f>0.00198*100</f>
         <v>0.19800000000000001</v>
       </c>
-      <c r="EI5">
-        <f t="shared" si="9"/>
+      <c r="EK5" s="8">
+        <f t="shared" si="11"/>
         <v>29.4925</v>
       </c>
-      <c r="EJ5">
-        <f t="shared" si="10"/>
+      <c r="EL5" s="8">
+        <f t="shared" si="12"/>
         <v>4.3474500000000003</v>
       </c>
-      <c r="EL5" s="2">
+      <c r="EM5" s="8">
+        <f t="shared" si="13"/>
+        <v>7.3758308345568802</v>
+      </c>
+      <c r="EN5" s="8">
+        <f t="shared" si="14"/>
+        <v>1.041214735297191</v>
+      </c>
+      <c r="EP5" s="9">
         <v>0.25900000000000001</v>
       </c>
-      <c r="EM5">
-        <f t="shared" si="11"/>
+      <c r="EQ5" s="8">
+        <f t="shared" si="15"/>
         <v>186.20999999999998</v>
       </c>
-      <c r="EN5">
-        <f t="shared" si="12"/>
+      <c r="ER5" s="8">
+        <f t="shared" si="16"/>
         <v>29.924500000000002</v>
       </c>
-      <c r="EP5" s="2">
+      <c r="ES5" s="8">
+        <f t="shared" si="17"/>
+        <v>56.186704833083205</v>
+      </c>
+      <c r="ET5" s="8">
+        <f t="shared" si="18"/>
+        <v>8.3148686399726124</v>
+      </c>
+      <c r="EV5" s="9">
         <f>0.00198*100</f>
         <v>0.19800000000000001</v>
       </c>
-      <c r="EQ5">
-        <f t="shared" si="13"/>
+      <c r="EW5" s="8">
+        <f t="shared" si="19"/>
         <v>214.625</v>
       </c>
-      <c r="ER5">
-        <f t="shared" si="14"/>
+      <c r="EX5" s="8">
+        <f t="shared" si="20"/>
         <v>36.843499999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY5" s="8">
+        <f t="shared" si="21"/>
+        <v>88.777256377970929</v>
+      </c>
+      <c r="EZ5" s="8">
+        <f t="shared" si="22"/>
+        <v>11.054200310289295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>7.3499999999999996E-2</v>
       </c>
@@ -2885,54 +3070,86 @@
       <c r="EB6">
         <v>5.0739999999999998</v>
       </c>
-      <c r="ED6" s="2">
+      <c r="ED6" s="9">
         <v>0.35499999999999998</v>
       </c>
-      <c r="EE6">
-        <f t="shared" si="15"/>
+      <c r="EE6" s="8">
+        <f t="shared" si="23"/>
         <v>44.704999999999998</v>
       </c>
-      <c r="EF6">
+      <c r="EF6" s="8">
         <f t="shared" si="8"/>
         <v>3.9573999999999998</v>
       </c>
-      <c r="EH6" s="2">
+      <c r="EG6" s="8">
+        <f t="shared" si="9"/>
+        <v>9.5643263223292863</v>
+      </c>
+      <c r="EH6" s="8">
+        <f t="shared" si="10"/>
+        <v>0.38254476862192216</v>
+      </c>
+      <c r="EJ6" s="9">
         <f>0.0025*100</f>
         <v>0.25</v>
       </c>
-      <c r="EI6">
-        <f t="shared" si="9"/>
+      <c r="EK6" s="8">
+        <f t="shared" si="11"/>
         <v>29.71</v>
       </c>
-      <c r="EJ6">
-        <f t="shared" si="10"/>
+      <c r="EL6" s="8">
+        <f t="shared" si="12"/>
         <v>4.3503999999999996</v>
       </c>
-      <c r="EL6" s="2">
+      <c r="EM6" s="8">
+        <f t="shared" si="13"/>
+        <v>7.3553247379024782</v>
+      </c>
+      <c r="EN6" s="8">
+        <f t="shared" si="14"/>
+        <v>1.023324933733174</v>
+      </c>
+      <c r="EP6" s="9">
         <v>0.35499999999999998</v>
       </c>
-      <c r="EM6">
-        <f t="shared" si="11"/>
+      <c r="EQ6" s="8">
+        <f t="shared" si="15"/>
         <v>192.69499999999999</v>
       </c>
-      <c r="EN6">
-        <f t="shared" si="12"/>
+      <c r="ER6" s="8">
+        <f t="shared" si="16"/>
         <v>29.9495</v>
       </c>
-      <c r="EP6" s="2">
+      <c r="ES6" s="8">
+        <f t="shared" si="17"/>
+        <v>56.915024817705167</v>
+      </c>
+      <c r="ET6" s="8">
+        <f t="shared" si="18"/>
+        <v>7.5653354519148728</v>
+      </c>
+      <c r="EV6" s="9">
         <f>0.0025*100</f>
         <v>0.25</v>
       </c>
-      <c r="EQ6">
-        <f t="shared" si="13"/>
+      <c r="EW6" s="8">
+        <f t="shared" si="19"/>
         <v>216.285</v>
       </c>
-      <c r="ER6">
-        <f t="shared" si="14"/>
+      <c r="EX6" s="8">
+        <f t="shared" si="20"/>
         <v>37.019500000000001</v>
       </c>
-    </row>
-    <row r="7" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY6" s="8">
+        <f t="shared" si="21"/>
+        <v>87.914586104923501</v>
+      </c>
+      <c r="EZ6" s="8">
+        <f t="shared" si="22"/>
+        <v>10.997631767794365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>9.11E-2</v>
       </c>
@@ -3251,54 +3468,86 @@
       <c r="EB7">
         <v>5.0952000000000002</v>
       </c>
-      <c r="ED7" s="2">
+      <c r="ED7" s="9">
         <v>0.48699999999999999</v>
       </c>
-      <c r="EE7">
-        <f t="shared" si="15"/>
+      <c r="EE7" s="8">
+        <f t="shared" si="23"/>
         <v>45.692499999999995</v>
       </c>
-      <c r="EF7">
+      <c r="EF7" s="8">
         <f t="shared" si="8"/>
         <v>4.0868000000000002</v>
       </c>
-      <c r="EH7" s="2">
+      <c r="EG7" s="8">
+        <f t="shared" si="9"/>
+        <v>9.6809989412250292</v>
+      </c>
+      <c r="EH7" s="8">
+        <f t="shared" si="10"/>
+        <v>0.3364414064885593</v>
+      </c>
+      <c r="EJ7" s="9">
         <f>0.00312*100</f>
         <v>0.312</v>
       </c>
-      <c r="EI7">
-        <f t="shared" si="9"/>
+      <c r="EK7" s="8">
+        <f t="shared" si="11"/>
         <v>29.960999999999999</v>
       </c>
-      <c r="EJ7">
-        <f t="shared" si="10"/>
+      <c r="EL7" s="8">
+        <f t="shared" si="12"/>
         <v>4.3669500000000001</v>
       </c>
-      <c r="EL7" s="2">
+      <c r="EM7" s="8">
+        <f t="shared" si="13"/>
+        <v>7.3072414767818019</v>
+      </c>
+      <c r="EN7" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0299010267982063</v>
+      </c>
+      <c r="EP7" s="9">
         <v>0.48699999999999999</v>
       </c>
-      <c r="EM7">
-        <f t="shared" si="11"/>
+      <c r="EQ7" s="8">
+        <f t="shared" si="15"/>
         <v>198.96</v>
       </c>
-      <c r="EN7">
-        <f t="shared" si="12"/>
+      <c r="ER7" s="8">
+        <f t="shared" si="16"/>
         <v>30.2685</v>
       </c>
-      <c r="EP7" s="2">
+      <c r="ES7" s="8">
+        <f t="shared" si="17"/>
+        <v>57.544349852961183</v>
+      </c>
+      <c r="ET7" s="8">
+        <f t="shared" si="18"/>
+        <v>6.8695423792272958</v>
+      </c>
+      <c r="EV7" s="9">
         <f>0.00312*100</f>
         <v>0.312</v>
       </c>
-      <c r="EQ7">
-        <f t="shared" si="13"/>
+      <c r="EW7" s="8">
+        <f t="shared" si="19"/>
         <v>217.57500000000002</v>
       </c>
-      <c r="ER7">
-        <f t="shared" si="14"/>
+      <c r="EX7" s="8">
+        <f t="shared" si="20"/>
         <v>37.146999999999998</v>
       </c>
-    </row>
-    <row r="8" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY7" s="8">
+        <f t="shared" si="21"/>
+        <v>86.825641661896157</v>
+      </c>
+      <c r="EZ7" s="8">
+        <f t="shared" si="22"/>
+        <v>10.943184545643025</v>
+      </c>
+    </row>
+    <row r="8" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>9.9599999999999994E-2</v>
       </c>
@@ -3617,54 +3866,86 @@
       <c r="EB8">
         <v>5.1106999999999996</v>
       </c>
-      <c r="ED8" s="2">
+      <c r="ED8" s="9">
         <v>0.66900000000000004</v>
       </c>
-      <c r="EE8">
-        <f t="shared" si="15"/>
+      <c r="EE8" s="8">
+        <f t="shared" si="23"/>
         <v>46.670999999999999</v>
       </c>
-      <c r="EF8">
+      <c r="EF8" s="8">
         <f t="shared" si="8"/>
         <v>4.2343500000000001</v>
       </c>
-      <c r="EH8" s="2">
+      <c r="EG8" s="8">
+        <f t="shared" si="9"/>
+        <v>9.7057476785665653</v>
+      </c>
+      <c r="EH8" s="8">
+        <f t="shared" si="10"/>
+        <v>0.26240732649832793</v>
+      </c>
+      <c r="EJ8" s="9">
         <f>0.00395*100</f>
         <v>0.39500000000000002</v>
       </c>
-      <c r="EI8">
-        <f t="shared" si="9"/>
+      <c r="EK8" s="8">
+        <f t="shared" si="11"/>
         <v>30.116999999999997</v>
       </c>
-      <c r="EJ8">
-        <f t="shared" si="10"/>
+      <c r="EL8" s="8">
+        <f t="shared" si="12"/>
         <v>4.3835499999999996</v>
       </c>
-      <c r="EL8" s="2">
+      <c r="EM8" s="8">
+        <f t="shared" si="13"/>
+        <v>7.2520871478492452</v>
+      </c>
+      <c r="EN8" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0283453918795964</v>
+      </c>
+      <c r="EP8" s="9">
         <v>0.66900000000000004</v>
       </c>
-      <c r="EM8">
-        <f t="shared" si="11"/>
+      <c r="EQ8" s="8">
+        <f t="shared" si="15"/>
         <v>204.93</v>
       </c>
-      <c r="EN8">
-        <f t="shared" si="12"/>
+      <c r="ER8" s="8">
+        <f t="shared" si="16"/>
         <v>30.779999999999998</v>
       </c>
-      <c r="EP8" s="2">
+      <c r="ES8" s="8">
+        <f t="shared" si="17"/>
+        <v>57.855476836683351</v>
+      </c>
+      <c r="ET8" s="8">
+        <f t="shared" si="18"/>
+        <v>6.2027406845683908</v>
+      </c>
+      <c r="EV8" s="9">
         <f>0.00395*100</f>
         <v>0.39500000000000002</v>
       </c>
-      <c r="EQ8">
-        <f t="shared" si="13"/>
+      <c r="EW8" s="8">
+        <f t="shared" si="19"/>
         <v>218.43</v>
       </c>
-      <c r="ER8">
-        <f t="shared" si="14"/>
+      <c r="EX8" s="8">
+        <f t="shared" si="20"/>
         <v>37.332000000000001</v>
       </c>
-    </row>
-    <row r="9" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY8" s="8">
+        <f t="shared" si="21"/>
+        <v>85.277077811097584</v>
+      </c>
+      <c r="EZ8" s="8">
+        <f t="shared" si="22"/>
+        <v>10.914900274395531</v>
+      </c>
+    </row>
+    <row r="9" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>0.14599999999999999</v>
       </c>
@@ -3983,54 +4264,86 @@
       <c r="EB9">
         <v>5.0911</v>
       </c>
-      <c r="ED9" s="2">
+      <c r="ED9" s="9">
         <v>0.91800000000000004</v>
       </c>
-      <c r="EE9">
-        <f t="shared" si="15"/>
+      <c r="EE9" s="8">
+        <f t="shared" si="23"/>
         <v>47.660499999999999</v>
       </c>
-      <c r="EF9">
+      <c r="EF9" s="8">
         <f t="shared" si="8"/>
         <v>4.4622000000000002</v>
       </c>
-      <c r="EH9" s="2">
+      <c r="EG9" s="8">
+        <f t="shared" si="9"/>
+        <v>9.7347390565951599</v>
+      </c>
+      <c r="EH9" s="8">
+        <f t="shared" si="10"/>
+        <v>0.24267904730322276</v>
+      </c>
+      <c r="EJ9" s="9">
         <f>0.00498*100</f>
         <v>0.498</v>
       </c>
-      <c r="EI9">
-        <f t="shared" si="9"/>
+      <c r="EK9" s="8">
+        <f t="shared" si="11"/>
         <v>30.269500000000001</v>
       </c>
-      <c r="EJ9">
-        <f t="shared" si="10"/>
+      <c r="EL9" s="8">
+        <f t="shared" si="12"/>
         <v>4.3710000000000004</v>
       </c>
-      <c r="EL9" s="2">
+      <c r="EM9" s="8">
+        <f t="shared" si="13"/>
+        <v>7.2400663325690768</v>
+      </c>
+      <c r="EN9" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0183751862648616</v>
+      </c>
+      <c r="EP9" s="9">
         <v>0.91800000000000004</v>
       </c>
-      <c r="EM9">
-        <f t="shared" si="11"/>
+      <c r="EQ9" s="8">
+        <f t="shared" si="15"/>
         <v>210.88499999999999</v>
       </c>
-      <c r="EN9">
-        <f t="shared" si="12"/>
+      <c r="ER9" s="8">
+        <f t="shared" si="16"/>
         <v>31.436500000000002</v>
       </c>
-      <c r="EP9" s="2">
+      <c r="ES9" s="8">
+        <f t="shared" si="17"/>
+        <v>58.117106345722348</v>
+      </c>
+      <c r="ET9" s="8">
+        <f t="shared" si="18"/>
+        <v>5.715544112330833</v>
+      </c>
+      <c r="EV9" s="9">
         <f>0.00498*100</f>
         <v>0.498</v>
       </c>
-      <c r="EQ9">
-        <f t="shared" si="13"/>
+      <c r="EW9" s="8">
+        <f t="shared" si="19"/>
         <v>218.90500000000003</v>
       </c>
-      <c r="ER9">
-        <f t="shared" si="14"/>
+      <c r="EX9" s="8">
+        <f t="shared" si="20"/>
         <v>37.603000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY9" s="8">
+        <f t="shared" si="21"/>
+        <v>83.360818434082006</v>
+      </c>
+      <c r="EZ9" s="8">
+        <f t="shared" si="22"/>
+        <v>10.869645440399623</v>
+      </c>
+    </row>
+    <row r="10" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0.214</v>
       </c>
@@ -4349,54 +4662,86 @@
       <c r="EB10">
         <v>5.1310000000000002</v>
       </c>
-      <c r="ED10" s="2">
+      <c r="ED10" s="9">
         <v>1.26</v>
       </c>
-      <c r="EE10">
-        <f t="shared" si="15"/>
+      <c r="EE10" s="8">
+        <f t="shared" si="23"/>
         <v>48.657499999999999</v>
       </c>
-      <c r="EF10">
+      <c r="EF10" s="8">
         <f t="shared" si="8"/>
         <v>4.6858000000000004</v>
       </c>
-      <c r="EH10" s="2">
+      <c r="EG10" s="8">
+        <f t="shared" si="9"/>
+        <v>9.7502954057813138</v>
+      </c>
+      <c r="EH10" s="8">
+        <f t="shared" si="10"/>
+        <v>0.22415284963613508</v>
+      </c>
+      <c r="EJ10" s="9">
         <f>0.00627*100</f>
         <v>0.627</v>
       </c>
-      <c r="EI10">
-        <f t="shared" si="9"/>
+      <c r="EK10" s="8">
+        <f t="shared" si="11"/>
         <v>30.392499999999998</v>
       </c>
-      <c r="EJ10">
-        <f t="shared" si="10"/>
+      <c r="EL10" s="8">
+        <f t="shared" si="12"/>
         <v>4.4058000000000002</v>
       </c>
-      <c r="EL10" s="2">
+      <c r="EM10" s="8">
+        <f t="shared" si="13"/>
+        <v>7.2230957698205911</v>
+      </c>
+      <c r="EN10" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0255876754329696</v>
+      </c>
+      <c r="EP10" s="9">
         <v>1.26</v>
       </c>
-      <c r="EM10">
-        <f t="shared" si="11"/>
+      <c r="EQ10" s="8">
+        <f t="shared" si="15"/>
         <v>216.82999999999998</v>
       </c>
-      <c r="EN10">
-        <f t="shared" si="12"/>
+      <c r="ER10" s="8">
+        <f t="shared" si="16"/>
         <v>32.426499999999997</v>
       </c>
-      <c r="EP10" s="2">
+      <c r="ES10" s="8">
+        <f t="shared" si="17"/>
+        <v>58.138319549158133</v>
+      </c>
+      <c r="ET10" s="8">
+        <f t="shared" si="18"/>
+        <v>5.6066496680281723</v>
+      </c>
+      <c r="EV10" s="9">
         <f>0.00627*100</f>
         <v>0.627</v>
       </c>
-      <c r="EQ10">
-        <f t="shared" si="13"/>
+      <c r="EW10" s="8">
+        <f t="shared" si="19"/>
         <v>218.57999999999998</v>
       </c>
-      <c r="ER10">
-        <f t="shared" si="14"/>
+      <c r="EX10" s="8">
+        <f t="shared" si="20"/>
         <v>37.845500000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY10" s="8">
+        <f t="shared" si="21"/>
+        <v>81.04857925960215</v>
+      </c>
+      <c r="EZ10" s="8">
+        <f t="shared" si="22"/>
+        <v>10.956619574485567</v>
+      </c>
+    </row>
+    <row r="11" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>0.313</v>
       </c>
@@ -4715,54 +5060,86 @@
       <c r="EB11">
         <v>5.1256000000000004</v>
       </c>
-      <c r="ED11" s="2">
+      <c r="ED11" s="9">
         <v>1.73</v>
       </c>
-      <c r="EE11">
-        <f t="shared" si="15"/>
+      <c r="EE11" s="8">
+        <f t="shared" si="23"/>
         <v>49.669499999999999</v>
       </c>
-      <c r="EF11">
+      <c r="EF11" s="8">
         <f t="shared" si="8"/>
         <v>4.93</v>
       </c>
-      <c r="EH11" s="2">
+      <c r="EG11" s="8">
+        <f t="shared" si="9"/>
+        <v>9.8054497347138572</v>
+      </c>
+      <c r="EH11" s="8">
+        <f t="shared" si="10"/>
+        <v>0.22938543981691586</v>
+      </c>
+      <c r="EJ11" s="9">
         <f>0.00788*100</f>
         <v>0.78800000000000003</v>
       </c>
-      <c r="EI11">
-        <f t="shared" si="9"/>
+      <c r="EK11" s="8">
+        <f t="shared" si="11"/>
         <v>30.439499999999999</v>
       </c>
-      <c r="EJ11">
-        <f t="shared" si="10"/>
+      <c r="EL11" s="8">
+        <f t="shared" si="12"/>
         <v>4.4116</v>
       </c>
-      <c r="EL11" s="2">
+      <c r="EM11" s="8">
+        <f t="shared" si="13"/>
+        <v>7.1368287425158403</v>
+      </c>
+      <c r="EN11" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0097484835343913</v>
+      </c>
+      <c r="EP11" s="9">
         <v>1.73</v>
       </c>
-      <c r="EM11">
-        <f t="shared" si="11"/>
+      <c r="EQ11" s="8">
+        <f t="shared" si="15"/>
         <v>222.83500000000001</v>
       </c>
-      <c r="EN11">
-        <f t="shared" si="12"/>
+      <c r="ER11" s="8">
+        <f t="shared" si="16"/>
         <v>33.602499999999999</v>
       </c>
-      <c r="EP11" s="2">
+      <c r="ES11" s="8">
+        <f t="shared" si="17"/>
+        <v>58.201959159464693</v>
+      </c>
+      <c r="ET11" s="8">
+        <f t="shared" si="18"/>
+        <v>5.6420050070874579</v>
+      </c>
+      <c r="EV11" s="9">
         <f>0.00788*100</f>
         <v>0.78800000000000003</v>
       </c>
-      <c r="EQ11">
-        <f t="shared" si="13"/>
+      <c r="EW11" s="8">
+        <f t="shared" si="19"/>
         <v>217.29500000000002</v>
       </c>
-      <c r="ER11">
-        <f t="shared" si="14"/>
+      <c r="EX11" s="8">
+        <f t="shared" si="20"/>
         <v>38.118499999999997</v>
       </c>
-    </row>
-    <row r="12" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY11" s="8">
+        <f t="shared" si="21"/>
+        <v>77.972664761440484</v>
+      </c>
+      <c r="EZ11" s="8">
+        <f t="shared" si="22"/>
+        <v>11.086727222223907</v>
+      </c>
+    </row>
+    <row r="12" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0.46600000000000003</v>
       </c>
@@ -5081,54 +5458,86 @@
       <c r="EB12">
         <v>5.1727999999999996</v>
       </c>
-      <c r="ED12" s="2">
+      <c r="ED12" s="9">
         <v>2.37</v>
       </c>
-      <c r="EE12">
-        <f t="shared" si="15"/>
+      <c r="EE12" s="8">
+        <f t="shared" si="23"/>
         <v>50.759</v>
       </c>
-      <c r="EF12">
+      <c r="EF12" s="8">
         <f t="shared" si="8"/>
         <v>5.1669499999999999</v>
       </c>
-      <c r="EH12" s="2">
+      <c r="EG12" s="8">
+        <f t="shared" si="9"/>
+        <v>9.8301984720553417</v>
+      </c>
+      <c r="EH12" s="8">
+        <f t="shared" si="10"/>
+        <v>0.26735707396663355</v>
+      </c>
+      <c r="EJ12" s="9">
         <f>0.00994*100</f>
         <v>0.99399999999999988</v>
       </c>
-      <c r="EI12">
-        <f t="shared" si="9"/>
+      <c r="EK12" s="8">
+        <f t="shared" si="11"/>
         <v>30.454999999999998</v>
       </c>
-      <c r="EJ12">
-        <f t="shared" si="10"/>
+      <c r="EL12" s="8">
+        <f t="shared" si="12"/>
         <v>4.4609499999999995</v>
       </c>
-      <c r="EL12" s="2">
+      <c r="EM12" s="8">
+        <f t="shared" si="13"/>
+        <v>7.0753104525526034</v>
+      </c>
+      <c r="EN12" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0067079243752899</v>
+      </c>
+      <c r="EP12" s="9">
         <v>2.37</v>
       </c>
-      <c r="EM12">
-        <f t="shared" si="11"/>
+      <c r="EQ12" s="8">
+        <f t="shared" si="15"/>
         <v>229.01499999999999</v>
       </c>
-      <c r="EN12">
-        <f t="shared" si="12"/>
+      <c r="ER12" s="8">
+        <f t="shared" si="16"/>
         <v>35.118000000000002</v>
       </c>
-      <c r="EP12" s="2">
+      <c r="ES12" s="8">
+        <f t="shared" si="17"/>
+        <v>58.230243430712406</v>
+      </c>
+      <c r="ET12" s="8">
+        <f t="shared" si="18"/>
+        <v>5.9807091552758065</v>
+      </c>
+      <c r="EV12" s="9">
         <f>0.00994*100</f>
         <v>0.99399999999999988</v>
       </c>
-      <c r="EQ12">
-        <f t="shared" si="13"/>
+      <c r="EW12" s="8">
+        <f t="shared" si="19"/>
         <v>215.255</v>
       </c>
-      <c r="ER12">
-        <f t="shared" si="14"/>
+      <c r="EX12" s="8">
+        <f t="shared" si="20"/>
         <v>38.408500000000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY12" s="8">
+        <f t="shared" si="21"/>
+        <v>74.027008922419725</v>
+      </c>
+      <c r="EZ12" s="8">
+        <f t="shared" si="22"/>
+        <v>11.226734364898789</v>
+      </c>
+    </row>
+    <row r="13" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>0.68300000000000005</v>
       </c>
@@ -5447,54 +5856,86 @@
       <c r="EB13">
         <v>5.2005999999999997</v>
       </c>
-      <c r="ED13" s="2">
+      <c r="ED13" s="9">
         <v>3.26</v>
       </c>
-      <c r="EE13">
-        <f t="shared" si="15"/>
+      <c r="EE13" s="8">
+        <f t="shared" si="23"/>
         <v>51.845500000000001</v>
       </c>
-      <c r="EF13">
+      <c r="EF13" s="8">
         <f t="shared" si="8"/>
         <v>5.4272500000000008</v>
       </c>
-      <c r="EH13" s="2">
+      <c r="EG13" s="8">
+        <f t="shared" si="9"/>
+        <v>9.8648467043334414</v>
+      </c>
+      <c r="EH13" s="8">
+        <f t="shared" si="10"/>
+        <v>0.30907637405663996</v>
+      </c>
+      <c r="EJ13" s="9">
         <f>0.0125*100</f>
         <v>1.25</v>
       </c>
-      <c r="EI13">
-        <f t="shared" si="9"/>
+      <c r="EK13" s="8">
+        <f t="shared" si="11"/>
         <v>30.375</v>
       </c>
-      <c r="EJ13">
-        <f t="shared" si="10"/>
+      <c r="EL13" s="8">
+        <f t="shared" si="12"/>
         <v>4.4914500000000004</v>
       </c>
-      <c r="EL13" s="2">
+      <c r="EM13" s="8">
+        <f t="shared" si="13"/>
+        <v>6.9607591540003595</v>
+      </c>
+      <c r="EN13" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0028895477568747</v>
+      </c>
+      <c r="EP13" s="9">
         <v>3.26</v>
       </c>
-      <c r="EM13">
-        <f t="shared" si="11"/>
+      <c r="EQ13" s="8">
+        <f t="shared" si="15"/>
         <v>235.435</v>
       </c>
-      <c r="EN13">
-        <f t="shared" si="12"/>
+      <c r="ER13" s="8">
+        <f t="shared" si="16"/>
         <v>36.938000000000002</v>
       </c>
-      <c r="EP13" s="2">
+      <c r="ES13" s="8">
+        <f t="shared" si="17"/>
+        <v>58.371664786949381</v>
+      </c>
+      <c r="ET13" s="8">
+        <f t="shared" si="18"/>
+        <v>6.6680169465891428</v>
+      </c>
+      <c r="EV13" s="9">
         <f>0.0125*100</f>
         <v>1.25</v>
       </c>
-      <c r="EQ13">
-        <f t="shared" si="13"/>
+      <c r="EW13" s="8">
+        <f t="shared" si="19"/>
         <v>211.89499999999998</v>
       </c>
-      <c r="ER13">
-        <f t="shared" si="14"/>
+      <c r="EX13" s="8">
+        <f t="shared" si="20"/>
         <v>38.686</v>
       </c>
-    </row>
-    <row r="14" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY13" s="8">
+        <f t="shared" si="21"/>
+        <v>69.176256403480039</v>
+      </c>
+      <c r="EZ13" s="8">
+        <f t="shared" si="22"/>
+        <v>11.358963332980707</v>
+      </c>
+    </row>
+    <row r="14" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>0.996</v>
       </c>
@@ -5813,54 +6254,86 @@
       <c r="EB14">
         <v>5.2298</v>
       </c>
-      <c r="ED14" s="2">
+      <c r="ED14" s="9">
         <v>4.47</v>
       </c>
-      <c r="EE14">
-        <f t="shared" si="15"/>
+      <c r="EE14" s="8">
+        <f t="shared" si="23"/>
         <v>52.978499999999997</v>
       </c>
-      <c r="EF14">
+      <c r="EF14" s="8">
         <f t="shared" si="8"/>
         <v>5.6845499999999998</v>
       </c>
-      <c r="EH14" s="2">
+      <c r="EG14" s="8">
+        <f t="shared" si="9"/>
+        <v>9.9256578875156052</v>
+      </c>
+      <c r="EH14" s="8">
+        <f t="shared" si="10"/>
+        <v>0.3638064389204787</v>
+      </c>
+      <c r="EJ14" s="9">
         <f>0.0158*100</f>
         <v>1.58</v>
       </c>
-      <c r="EI14">
-        <f t="shared" si="9"/>
+      <c r="EK14" s="8">
+        <f t="shared" si="11"/>
         <v>30.222499999999997</v>
       </c>
-      <c r="EJ14">
-        <f t="shared" si="10"/>
+      <c r="EL14" s="8">
+        <f t="shared" si="12"/>
         <v>4.5230999999999995</v>
       </c>
-      <c r="EL14" s="2">
+      <c r="EM14" s="8">
+        <f t="shared" si="13"/>
+        <v>6.8313586130432569</v>
+      </c>
+      <c r="EN14" s="8">
+        <f t="shared" si="14"/>
+        <v>0.99942472452907005</v>
+      </c>
+      <c r="EP14" s="9">
         <v>4.47</v>
       </c>
-      <c r="EM14">
-        <f t="shared" si="11"/>
+      <c r="EQ14" s="8">
+        <f t="shared" si="15"/>
         <v>242.15500000000003</v>
       </c>
-      <c r="EN14">
-        <f t="shared" si="12"/>
+      <c r="ER14" s="8">
+        <f t="shared" si="16"/>
         <v>39.090000000000003</v>
       </c>
-      <c r="EP14" s="2">
+      <c r="ES14" s="8">
+        <f t="shared" si="17"/>
+        <v>58.696933906295094</v>
+      </c>
+      <c r="ET14" s="8">
+        <f t="shared" si="18"/>
+        <v>7.6183684605038327</v>
+      </c>
+      <c r="EV14" s="9">
         <f>0.0158*100</f>
         <v>1.58</v>
       </c>
-      <c r="EQ14">
-        <f t="shared" si="13"/>
+      <c r="EW14" s="8">
+        <f t="shared" si="19"/>
         <v>207.12</v>
       </c>
-      <c r="ER14">
-        <f t="shared" si="14"/>
+      <c r="EX14" s="8">
+        <f t="shared" si="20"/>
         <v>38.923999999999999</v>
       </c>
-    </row>
-    <row r="15" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY14" s="8">
+        <f t="shared" si="21"/>
+        <v>63.116351288711265</v>
+      </c>
+      <c r="EZ14" s="8">
+        <f t="shared" si="22"/>
+        <v>11.446644573847841</v>
+      </c>
+    </row>
+    <row r="15" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1.46</v>
       </c>
@@ -6179,54 +6652,86 @@
       <c r="EB15">
         <v>5.2870999999999997</v>
       </c>
-      <c r="ED15" s="2">
+      <c r="ED15" s="9">
         <v>6.14</v>
       </c>
-      <c r="EE15">
-        <f t="shared" si="15"/>
+      <c r="EE15" s="8">
+        <f t="shared" si="23"/>
         <v>54.123999999999995</v>
       </c>
-      <c r="EF15">
+      <c r="EF15" s="8">
         <f t="shared" si="8"/>
         <v>5.9522499999999994</v>
       </c>
-      <c r="EH15" s="2">
+      <c r="EG15" s="8">
+        <f t="shared" si="9"/>
+        <v>10.053644214910353</v>
+      </c>
+      <c r="EH15" s="8">
+        <f t="shared" si="10"/>
+        <v>0.42490046481499655</v>
+      </c>
+      <c r="EJ15" s="9">
         <f>0.0198*100</f>
         <v>1.9800000000000002</v>
       </c>
-      <c r="EI15">
-        <f t="shared" si="9"/>
+      <c r="EK15" s="8">
+        <f t="shared" si="11"/>
         <v>29.939500000000002</v>
       </c>
-      <c r="EJ15">
-        <f t="shared" si="10"/>
+      <c r="EL15" s="8">
+        <f t="shared" si="12"/>
         <v>4.5683999999999996</v>
       </c>
-      <c r="EL15" s="2">
+      <c r="EM15" s="8">
+        <f t="shared" si="13"/>
+        <v>6.6856946161187976</v>
+      </c>
+      <c r="EN15" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0163952872775457</v>
+      </c>
+      <c r="EP15" s="9">
         <v>6.14</v>
       </c>
-      <c r="EM15">
-        <f t="shared" si="11"/>
+      <c r="EQ15" s="8">
+        <f t="shared" si="15"/>
         <v>249.25</v>
       </c>
-      <c r="EN15">
-        <f t="shared" si="12"/>
+      <c r="ER15" s="8">
+        <f t="shared" si="16"/>
         <v>41.585000000000001</v>
       </c>
-      <c r="EP15" s="2">
+      <c r="ES15" s="8">
+        <f t="shared" si="17"/>
+        <v>59.283832534680222</v>
+      </c>
+      <c r="ET15" s="8">
+        <f t="shared" si="18"/>
+        <v>8.8529769004555714</v>
+      </c>
+      <c r="EV15" s="9">
         <f>0.0198*100</f>
         <v>1.9800000000000002</v>
       </c>
-      <c r="EQ15">
-        <f t="shared" si="13"/>
+      <c r="EW15" s="8">
+        <f t="shared" si="19"/>
         <v>200.64999999999998</v>
       </c>
-      <c r="ER15">
-        <f t="shared" si="14"/>
+      <c r="EX15" s="8">
+        <f t="shared" si="20"/>
         <v>39.128</v>
       </c>
-    </row>
-    <row r="16" spans="1:148" x14ac:dyDescent="0.35">
+      <c r="EY15" s="8">
+        <f t="shared" si="21"/>
+        <v>55.70587222187617</v>
+      </c>
+      <c r="EZ15" s="8">
+        <f t="shared" si="22"/>
+        <v>11.439573506035975</v>
+      </c>
+    </row>
+    <row r="16" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2.15</v>
       </c>
@@ -6545,54 +7050,86 @@
       <c r="EB16">
         <v>5.3532000000000002</v>
       </c>
-      <c r="ED16" s="2">
+      <c r="ED16" s="9">
         <v>8.43</v>
       </c>
-      <c r="EE16">
-        <f t="shared" si="15"/>
+      <c r="EE16" s="8">
+        <f t="shared" si="23"/>
         <v>55.279499999999999</v>
       </c>
-      <c r="EF16">
+      <c r="EF16" s="8">
         <f t="shared" si="8"/>
         <v>6.2625999999999999</v>
       </c>
-      <c r="EH16" s="2">
+      <c r="EG16" s="8">
+        <f t="shared" si="9"/>
+        <v>10.180216328742766</v>
+      </c>
+      <c r="EH16" s="8">
+        <f t="shared" si="10"/>
+        <v>0.54715922728215016</v>
+      </c>
+      <c r="EJ16" s="9">
         <f>0.025*100</f>
         <v>2.5</v>
       </c>
-      <c r="EI16">
-        <f t="shared" si="9"/>
+      <c r="EK16" s="8">
+        <f t="shared" si="11"/>
         <v>29.476500000000001</v>
       </c>
-      <c r="EJ16">
-        <f t="shared" si="10"/>
+      <c r="EL16" s="8">
+        <f t="shared" si="12"/>
         <v>4.6253500000000001</v>
       </c>
-      <c r="EL16" s="2">
+      <c r="EM16" s="8">
+        <f t="shared" si="13"/>
+        <v>6.4891189309489317</v>
+      </c>
+      <c r="EN16" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0293353413732549</v>
+      </c>
+      <c r="EP16" s="9">
         <v>8.43</v>
       </c>
-      <c r="EM16">
-        <f t="shared" si="11"/>
+      <c r="EQ16" s="8">
+        <f t="shared" si="15"/>
         <v>256.79500000000002</v>
       </c>
-      <c r="EN16">
-        <f t="shared" si="12"/>
+      <c r="ER16" s="8">
+        <f t="shared" si="16"/>
         <v>44.435500000000005</v>
       </c>
-      <c r="EP16" s="2">
+      <c r="ES16" s="8">
+        <f t="shared" si="17"/>
+        <v>60.196000282410886</v>
+      </c>
+      <c r="ET16" s="8">
+        <f t="shared" si="18"/>
+        <v>10.338608247728484</v>
+      </c>
+      <c r="EV16" s="9">
         <f>0.025*100</f>
         <v>2.5</v>
       </c>
-      <c r="EQ16">
-        <f t="shared" si="13"/>
+      <c r="EW16" s="8">
+        <f t="shared" si="19"/>
         <v>192.21499999999997</v>
       </c>
-      <c r="ER16">
-        <f t="shared" si="14"/>
+      <c r="EX16" s="8">
+        <f t="shared" si="20"/>
         <v>39.185500000000005</v>
       </c>
-    </row>
-    <row r="17" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY16" s="8">
+        <f t="shared" si="21"/>
+        <v>47.001387745469934</v>
+      </c>
+      <c r="EZ16" s="8">
+        <f t="shared" si="22"/>
+        <v>11.235219646273045</v>
+      </c>
+    </row>
+    <row r="17" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>3.16</v>
       </c>
@@ -6911,54 +7448,86 @@
       <c r="EB17">
         <v>5.4428999999999998</v>
       </c>
-      <c r="ED17" s="2">
+      <c r="ED17" s="9">
         <v>11.6</v>
       </c>
-      <c r="EE17">
-        <f t="shared" si="15"/>
+      <c r="EE17" s="8">
+        <f t="shared" si="23"/>
         <v>56.42</v>
       </c>
-      <c r="EF17">
+      <c r="EF17" s="8">
         <f t="shared" si="8"/>
         <v>6.5781999999999998</v>
       </c>
-      <c r="EH17" s="2">
+      <c r="EG17" s="8">
+        <f t="shared" si="9"/>
+        <v>10.363356985070036</v>
+      </c>
+      <c r="EH17" s="8">
+        <f t="shared" si="10"/>
+        <v>0.63851742341145279</v>
+      </c>
+      <c r="EJ17" s="9">
         <f>0.0315*100</f>
         <v>3.15</v>
       </c>
-      <c r="EI17">
-        <f t="shared" si="9"/>
+      <c r="EK17" s="8">
+        <f t="shared" si="11"/>
         <v>28.756500000000003</v>
       </c>
-      <c r="EJ17">
-        <f t="shared" si="10"/>
+      <c r="EL17" s="8">
+        <f t="shared" si="12"/>
         <v>4.6973000000000003</v>
       </c>
-      <c r="EL17" s="2">
+      <c r="EM17" s="8">
+        <f t="shared" si="13"/>
+        <v>6.2062762184742981</v>
+      </c>
+      <c r="EN17" s="8">
+        <f t="shared" si="14"/>
+        <v>1.0544376321053803</v>
+      </c>
+      <c r="EP17" s="9">
         <v>11.6</v>
       </c>
-      <c r="EM17">
-        <f t="shared" si="11"/>
+      <c r="EQ17" s="8">
+        <f t="shared" si="15"/>
         <v>264.88499999999999</v>
       </c>
-      <c r="EN17">
-        <f t="shared" si="12"/>
+      <c r="ER17" s="8">
+        <f t="shared" si="16"/>
         <v>47.628</v>
       </c>
-      <c r="EP17" s="2">
+      <c r="ES17" s="8">
+        <f t="shared" si="17"/>
+        <v>61.412223946051832</v>
+      </c>
+      <c r="ET17" s="8">
+        <f t="shared" si="18"/>
+        <v>12.088697531165208</v>
+      </c>
+      <c r="EV17" s="9">
         <f>0.0315*100</f>
         <v>3.15</v>
       </c>
-      <c r="EQ17">
-        <f t="shared" si="13"/>
+      <c r="EW17" s="8">
+        <f t="shared" si="19"/>
         <v>181.39500000000001</v>
       </c>
-      <c r="ER17">
-        <f t="shared" si="14"/>
+      <c r="EX17" s="8">
+        <f t="shared" si="20"/>
         <v>38.969499999999996</v>
       </c>
-    </row>
-    <row r="18" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY17" s="8">
+        <f t="shared" si="21"/>
+        <v>37.031182130739452</v>
+      </c>
+      <c r="EZ17" s="8">
+        <f t="shared" si="22"/>
+        <v>10.709132201070291</v>
+      </c>
+    </row>
+    <row r="18" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>4.6500000000000004</v>
       </c>
@@ -7277,54 +7846,86 @@
       <c r="EB18">
         <v>5.6021000000000001</v>
       </c>
-      <c r="ED18" s="2">
+      <c r="ED18" s="9">
         <v>15.9</v>
       </c>
-      <c r="EE18">
-        <f t="shared" si="15"/>
+      <c r="EE18" s="8">
+        <f t="shared" si="23"/>
         <v>57.441500000000005</v>
       </c>
-      <c r="EF18">
+      <c r="EF18" s="8">
         <f t="shared" si="8"/>
         <v>6.9471500000000006</v>
       </c>
-      <c r="EH18" s="2">
+      <c r="EG18" s="8">
+        <f t="shared" si="9"/>
+        <v>10.639835736513982</v>
+      </c>
+      <c r="EH18" s="8">
+        <f t="shared" si="10"/>
+        <v>0.7111372898393109</v>
+      </c>
+      <c r="EJ18" s="9">
         <f>0.0397*100</f>
         <v>3.9699999999999998</v>
       </c>
-      <c r="EI18">
-        <f t="shared" si="9"/>
+      <c r="EK18" s="8">
+        <f t="shared" si="11"/>
         <v>27.650500000000001</v>
       </c>
-      <c r="EJ18">
-        <f t="shared" si="10"/>
+      <c r="EL18" s="8">
+        <f t="shared" si="12"/>
         <v>4.8016000000000005</v>
       </c>
-      <c r="EL18" s="2">
+      <c r="EM18" s="8">
+        <f t="shared" si="13"/>
+        <v>5.7961542853861179</v>
+      </c>
+      <c r="EN18" s="8">
+        <f t="shared" si="14"/>
+        <v>1.1320779566796577</v>
+      </c>
+      <c r="EP18" s="9">
         <v>15.9</v>
       </c>
-      <c r="EM18">
-        <f t="shared" si="11"/>
+      <c r="EQ18" s="8">
+        <f t="shared" si="15"/>
         <v>273.52999999999997</v>
       </c>
-      <c r="EN18">
-        <f t="shared" si="12"/>
+      <c r="ER18" s="8">
+        <f t="shared" si="16"/>
         <v>51.159500000000001</v>
       </c>
-      <c r="EP18" s="2">
+      <c r="ES18" s="8">
+        <f t="shared" si="17"/>
+        <v>63.088067017463786</v>
+      </c>
+      <c r="ET18" s="8">
+        <f t="shared" si="18"/>
+        <v>14.045261994708406</v>
+      </c>
+      <c r="EV18" s="9">
         <f>0.0397*100</f>
         <v>3.9699999999999998</v>
       </c>
-      <c r="EQ18">
-        <f t="shared" si="13"/>
+      <c r="EW18" s="8">
+        <f t="shared" si="19"/>
         <v>167.87</v>
       </c>
-      <c r="ER18">
-        <f t="shared" si="14"/>
+      <c r="EX18" s="8">
+        <f t="shared" si="20"/>
         <v>38.370999999999995</v>
       </c>
-    </row>
-    <row r="19" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY18" s="8">
+        <f t="shared" si="21"/>
+        <v>25.950818869546147</v>
+      </c>
+      <c r="EZ18" s="8">
+        <f t="shared" si="22"/>
+        <v>9.7128187463784332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>6.84</v>
       </c>
@@ -7643,54 +8244,86 @@
       <c r="EB19">
         <v>5.8696000000000002</v>
       </c>
-      <c r="ED19" s="2">
+      <c r="ED19" s="9">
         <v>21.8</v>
       </c>
-      <c r="EE19">
-        <f t="shared" si="15"/>
+      <c r="EE19" s="8">
+        <f t="shared" si="23"/>
         <v>58.349000000000004</v>
       </c>
-      <c r="EF19">
+      <c r="EF19" s="8">
         <f t="shared" si="8"/>
         <v>7.4512499999999999</v>
       </c>
-      <c r="EH19" s="2">
+      <c r="EG19" s="8">
+        <f t="shared" si="9"/>
+        <v>11.086020115442642</v>
+      </c>
+      <c r="EH19" s="8">
+        <f t="shared" si="10"/>
+        <v>0.86415519728807988</v>
+      </c>
+      <c r="EJ19" s="9">
         <f>0.05*100</f>
         <v>5</v>
       </c>
-      <c r="EI19">
-        <f t="shared" si="9"/>
+      <c r="EK19" s="8">
+        <f t="shared" si="11"/>
         <v>25.945999999999998</v>
       </c>
-      <c r="EJ19">
-        <f t="shared" si="10"/>
+      <c r="EL19" s="8">
+        <f t="shared" si="12"/>
         <v>5.0031499999999998</v>
       </c>
-      <c r="EL19" s="2">
+      <c r="EM19" s="8">
+        <f t="shared" si="13"/>
+        <v>5.2849160825882677</v>
+      </c>
+      <c r="EN19" s="8">
+        <f t="shared" si="14"/>
+        <v>1.2253453411181716</v>
+      </c>
+      <c r="EP19" s="9">
         <v>21.8</v>
       </c>
-      <c r="EM19">
-        <f t="shared" si="11"/>
+      <c r="EQ19" s="8">
+        <f t="shared" si="15"/>
         <v>282.76</v>
       </c>
-      <c r="EN19">
-        <f t="shared" si="12"/>
+      <c r="ER19" s="8">
+        <f t="shared" si="16"/>
         <v>55.126999999999995</v>
       </c>
-      <c r="EP19" s="2">
+      <c r="ES19" s="8">
+        <f t="shared" si="17"/>
+        <v>65.364950852884746</v>
+      </c>
+      <c r="ET19" s="8">
+        <f t="shared" si="18"/>
+        <v>16.187088434922458</v>
+      </c>
+      <c r="EV19" s="9">
         <f>0.05*100</f>
         <v>5</v>
       </c>
-      <c r="EQ19">
-        <f t="shared" si="13"/>
+      <c r="EW19" s="8">
+        <f t="shared" si="19"/>
         <v>151.09</v>
       </c>
-      <c r="ER19">
-        <f t="shared" si="14"/>
+      <c r="EX19" s="8">
+        <f t="shared" si="20"/>
         <v>37.341999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY19" s="8">
+        <f t="shared" si="21"/>
+        <v>14.325983386839447</v>
+      </c>
+      <c r="EZ19" s="8">
+        <f t="shared" si="22"/>
+        <v>8.0143482579683507</v>
+      </c>
+    </row>
+    <row r="20" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>10</v>
       </c>
@@ -8009,54 +8642,86 @@
       <c r="EB20">
         <v>6.9840999999999998</v>
       </c>
-      <c r="ED20" s="2">
+      <c r="ED20" s="9">
         <v>29.9</v>
       </c>
-      <c r="EE20">
-        <f t="shared" si="15"/>
+      <c r="EE20" s="8">
+        <f t="shared" si="23"/>
         <v>59.17</v>
       </c>
-      <c r="EF20">
+      <c r="EF20" s="8">
         <f t="shared" si="8"/>
         <v>8.2597000000000005</v>
       </c>
-      <c r="EH20" s="2">
+      <c r="EG20" s="8">
+        <f t="shared" si="9"/>
+        <v>11.96141831055165</v>
+      </c>
+      <c r="EH20" s="8">
+        <f t="shared" si="10"/>
+        <v>0.98415121805543737</v>
+      </c>
+      <c r="EJ20" s="9">
         <f>0.0631*100</f>
         <v>6.3100000000000005</v>
       </c>
-      <c r="EI20">
-        <f t="shared" si="9"/>
+      <c r="EK20" s="8">
+        <f t="shared" si="11"/>
         <v>22.981999999999999</v>
       </c>
-      <c r="EJ20">
-        <f t="shared" si="10"/>
+      <c r="EL20" s="8">
+        <f t="shared" si="12"/>
         <v>5.6454500000000003</v>
       </c>
-      <c r="EL20" s="2">
+      <c r="EM20" s="8">
+        <f t="shared" si="13"/>
+        <v>4.0531360697612753</v>
+      </c>
+      <c r="EN20" s="8">
+        <f t="shared" si="14"/>
+        <v>1.893136985270744</v>
+      </c>
+      <c r="EP20" s="9">
         <v>29.9</v>
       </c>
-      <c r="EM20">
-        <f t="shared" si="11"/>
+      <c r="EQ20" s="8">
+        <f t="shared" si="15"/>
         <v>292.61500000000001</v>
       </c>
-      <c r="EN20">
-        <f t="shared" si="12"/>
+      <c r="ER20" s="8">
+        <f t="shared" si="16"/>
         <v>59.641000000000005</v>
       </c>
-      <c r="EP20" s="2">
+      <c r="ES20" s="8">
+        <f t="shared" si="17"/>
+        <v>68.242875452313484</v>
+      </c>
+      <c r="ET20" s="8">
+        <f t="shared" si="18"/>
+        <v>18.442759066907506</v>
+      </c>
+      <c r="EV20" s="9">
         <f>0.0631*100</f>
         <v>6.3100000000000005</v>
       </c>
-      <c r="EQ20">
-        <f t="shared" si="13"/>
+      <c r="EW20" s="8">
+        <f t="shared" si="19"/>
         <v>128.92000000000002</v>
       </c>
-      <c r="ER20">
-        <f t="shared" si="14"/>
+      <c r="EX20" s="8">
+        <f t="shared" si="20"/>
         <v>35.896000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY20" s="8">
+        <f t="shared" si="21"/>
+        <v>5.4447222151364283</v>
+      </c>
+      <c r="EZ20" s="8">
+        <f t="shared" si="22"/>
+        <v>4.9978307294265161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>14.799999999999999</v>
       </c>
@@ -8375,54 +9040,86 @@
       <c r="EB21">
         <v>8.4017999999999997</v>
       </c>
-      <c r="ED21" s="2">
+      <c r="ED21" s="9">
         <v>41.1</v>
       </c>
-      <c r="EE21">
-        <f t="shared" si="15"/>
+      <c r="EE21" s="8">
+        <f t="shared" si="23"/>
         <v>60.424499999999995</v>
       </c>
-      <c r="EF21">
+      <c r="EF21" s="8">
         <f t="shared" si="8"/>
         <v>7.6722999999999999</v>
       </c>
-      <c r="EH21" s="2">
+      <c r="EG21" s="8">
+        <f t="shared" si="9"/>
+        <v>13.014300307738406</v>
+      </c>
+      <c r="EH21" s="8">
+        <f t="shared" si="10"/>
+        <v>1.3015007414519555</v>
+      </c>
+      <c r="EJ21" s="9">
         <f>0.0795*100</f>
         <v>7.95</v>
       </c>
-      <c r="EI21">
-        <f t="shared" si="9"/>
+      <c r="EK21" s="8">
+        <f t="shared" si="11"/>
         <v>18.999000000000002</v>
       </c>
-      <c r="EJ21">
-        <f t="shared" si="10"/>
+      <c r="EL21" s="8">
+        <f t="shared" si="12"/>
         <v>6.4879499999999997</v>
       </c>
-      <c r="EL21" s="2">
+      <c r="EM21" s="8">
+        <f t="shared" si="13"/>
+        <v>2.7435743110037825</v>
+      </c>
+      <c r="EN21" s="8">
+        <f t="shared" si="14"/>
+        <v>2.706592626347748</v>
+      </c>
+      <c r="EP21" s="9">
         <v>41.1</v>
       </c>
-      <c r="EM21">
-        <f t="shared" si="11"/>
+      <c r="EQ21" s="8">
+        <f t="shared" si="15"/>
         <v>303.83</v>
       </c>
-      <c r="EN21">
-        <f t="shared" si="12"/>
+      <c r="ER21" s="8">
+        <f t="shared" si="16"/>
         <v>62.9255</v>
       </c>
-      <c r="EP21" s="2">
+      <c r="ES21" s="8">
+        <f t="shared" si="17"/>
+        <v>71.743054019187397</v>
+      </c>
+      <c r="ET21" s="8">
+        <f t="shared" si="18"/>
+        <v>20.741563212544996</v>
+      </c>
+      <c r="EV21" s="9">
         <f>0.0795*100</f>
         <v>7.95</v>
       </c>
-      <c r="EQ21">
-        <f t="shared" si="13"/>
+      <c r="EW21" s="8">
+        <f t="shared" si="19"/>
         <v>99.403499999999994</v>
       </c>
-      <c r="ER21">
-        <f t="shared" si="14"/>
+      <c r="EX21" s="8">
+        <f t="shared" si="20"/>
         <v>34.087500000000006</v>
       </c>
-    </row>
-    <row r="22" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY21" s="8">
+        <f t="shared" si="21"/>
+        <v>5.383203925173186</v>
+      </c>
+      <c r="EZ21" s="8">
+        <f t="shared" si="22"/>
+        <v>0.52538033842160625</v>
+      </c>
+    </row>
+    <row r="22" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21.6</v>
       </c>
@@ -8741,54 +9438,86 @@
       <c r="EB22">
         <v>9.7985000000000007</v>
       </c>
-      <c r="ED22" s="2">
+      <c r="ED22" s="9">
         <v>56.3</v>
       </c>
-      <c r="EE22">
-        <f t="shared" si="15"/>
+      <c r="EE22" s="8">
+        <f t="shared" si="23"/>
         <v>58.695499999999996</v>
       </c>
-      <c r="EF22">
+      <c r="EF22" s="8">
         <f t="shared" si="8"/>
         <v>6.4653999999999998</v>
       </c>
-      <c r="EH22" s="2">
+      <c r="EG22" s="8">
+        <f t="shared" si="9"/>
+        <v>15.69989186268494</v>
+      </c>
+      <c r="EH22" s="8">
+        <f t="shared" si="10"/>
+        <v>1.0547204748178474</v>
+      </c>
+      <c r="EJ22" s="9">
         <f>0.1*100</f>
         <v>10</v>
       </c>
-      <c r="EI22">
-        <f t="shared" si="9"/>
+      <c r="EK22" s="8">
+        <f t="shared" si="11"/>
         <v>14.6265</v>
       </c>
-      <c r="EJ22">
-        <f t="shared" si="10"/>
+      <c r="EL22" s="8">
+        <f t="shared" si="12"/>
         <v>7.2692500000000004</v>
       </c>
-      <c r="EL22" s="2">
+      <c r="EM22" s="8">
+        <f t="shared" si="13"/>
+        <v>0.92136013588607202</v>
+      </c>
+      <c r="EN22" s="8">
+        <f t="shared" si="14"/>
+        <v>3.5768996526321533</v>
+      </c>
+      <c r="EP22" s="9">
         <v>56.3</v>
       </c>
-      <c r="EM22">
-        <f t="shared" si="11"/>
+      <c r="EQ22" s="8">
+        <f t="shared" si="15"/>
         <v>312.56</v>
       </c>
-      <c r="EN22">
-        <f t="shared" si="12"/>
+      <c r="ER22" s="8">
+        <f t="shared" si="16"/>
         <v>66.43950000000001</v>
       </c>
-      <c r="EP22" s="2">
+      <c r="ES22" s="8">
+        <f t="shared" si="17"/>
+        <v>77.187776234323522</v>
+      </c>
+      <c r="ET22" s="8">
+        <f t="shared" si="18"/>
+        <v>23.391799428432176</v>
+      </c>
+      <c r="EV22" s="9">
         <f>0.1*100</f>
         <v>10</v>
       </c>
-      <c r="EQ22">
-        <f t="shared" si="13"/>
+      <c r="EW22" s="8">
+        <f t="shared" si="19"/>
         <v>69.238</v>
       </c>
-      <c r="ER22">
-        <f t="shared" si="14"/>
+      <c r="EX22" s="8">
+        <f t="shared" si="20"/>
         <v>31.016500000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY22" s="8">
+        <f t="shared" si="21"/>
+        <v>10.837118528464968</v>
+      </c>
+      <c r="EZ22" s="8">
+        <f t="shared" si="22"/>
+        <v>3.165717059372176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>31.7</v>
       </c>
@@ -9107,54 +9836,86 @@
       <c r="EB23">
         <v>9.9314</v>
       </c>
-      <c r="ED23" s="2">
+      <c r="ED23" s="9">
         <v>77.3</v>
       </c>
-      <c r="EE23">
-        <f t="shared" si="15"/>
+      <c r="EE23" s="8">
+        <f t="shared" si="23"/>
         <v>53.853999999999999</v>
       </c>
-      <c r="EF23">
+      <c r="EF23" s="8">
         <f t="shared" si="8"/>
         <v>5.1635</v>
       </c>
-      <c r="EH23" s="2">
+      <c r="EG23" s="8">
+        <f t="shared" si="9"/>
+        <v>19.121581576846626</v>
+      </c>
+      <c r="EH23" s="8">
+        <f t="shared" si="10"/>
+        <v>0.87921657172734946</v>
+      </c>
+      <c r="EJ23" s="9">
         <f>0.126*100</f>
         <v>12.6</v>
       </c>
-      <c r="EI23">
-        <f t="shared" si="9"/>
+      <c r="EK23" s="8">
+        <f t="shared" si="11"/>
         <v>10.945</v>
       </c>
-      <c r="EJ23">
-        <f t="shared" si="10"/>
+      <c r="EL23" s="8">
+        <f t="shared" si="12"/>
         <v>7.3743999999999996</v>
       </c>
-      <c r="EL23" s="2">
+      <c r="EM23" s="8">
+        <f t="shared" si="13"/>
+        <v>0.42850670939904772</v>
+      </c>
+      <c r="EN23" s="8">
+        <f t="shared" si="14"/>
+        <v>3.6161440789880062</v>
+      </c>
+      <c r="EP23" s="9">
         <v>77.3</v>
       </c>
-      <c r="EM23">
-        <f t="shared" si="11"/>
+      <c r="EQ23" s="8">
+        <f t="shared" si="15"/>
         <v>320.39</v>
       </c>
-      <c r="EN23">
-        <f t="shared" si="12"/>
+      <c r="ER23" s="8">
+        <f t="shared" si="16"/>
         <v>69.028999999999996</v>
       </c>
-      <c r="EP23" s="2">
+      <c r="ES23" s="8">
+        <f t="shared" si="17"/>
+        <v>83.424458044388842</v>
+      </c>
+      <c r="ET23" s="8">
+        <f t="shared" si="18"/>
+        <v>25.735858408065631</v>
+      </c>
+      <c r="EV23" s="9">
         <f>0.126*100</f>
         <v>12.6</v>
       </c>
-      <c r="EQ23">
-        <f t="shared" si="13"/>
+      <c r="EW23" s="8">
+        <f t="shared" si="19"/>
         <v>45.42</v>
       </c>
-      <c r="ER23">
-        <f t="shared" si="14"/>
+      <c r="EX23" s="8">
+        <f t="shared" si="20"/>
         <v>26.877000000000002</v>
       </c>
-    </row>
-    <row r="24" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY23" s="8">
+        <f t="shared" si="21"/>
+        <v>10.636300202608066</v>
+      </c>
+      <c r="EZ23" s="8">
+        <f t="shared" si="22"/>
+        <v>5.904341622907646</v>
+      </c>
+    </row>
+    <row r="24" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>46.5</v>
       </c>
@@ -9477,58 +10238,86 @@
       <c r="EB24">
         <v>9.2870000000000008</v>
       </c>
-      <c r="ED24" s="2">
+      <c r="ED24" s="9">
         <v>106</v>
       </c>
-      <c r="EE24">
-        <f t="shared" si="15"/>
+      <c r="EE24" s="8">
+        <f t="shared" si="23"/>
         <v>44.091499999999996</v>
       </c>
-      <c r="EF24">
+      <c r="EF24" s="8">
         <f t="shared" si="8"/>
         <v>2.47445</v>
       </c>
-      <c r="EH24" s="5">
+      <c r="EG24" s="8">
+        <f t="shared" si="9"/>
+        <v>25.909099569456295</v>
+      </c>
+      <c r="EH24" s="8">
+        <f t="shared" si="10"/>
+        <v>0.55543237662203304</v>
+      </c>
+      <c r="EJ24" s="9">
         <f>0.158*100</f>
         <v>15.8</v>
       </c>
-      <c r="EI24" s="6">
-        <f t="shared" si="9"/>
+      <c r="EK24" s="8">
+        <f t="shared" si="11"/>
         <v>7.8012499999999996</v>
       </c>
-      <c r="EJ24" s="6">
-        <f t="shared" si="10"/>
+      <c r="EL24" s="8">
+        <f t="shared" si="12"/>
         <v>7.1298000000000004</v>
       </c>
-      <c r="EK24">
-        <f>AVERAGE(EI24:EJ24)</f>
-        <v>7.4655249999999995</v>
-      </c>
-      <c r="EL24" s="2">
+      <c r="EM24" s="8">
+        <f t="shared" si="13"/>
+        <v>0.74394704448636617</v>
+      </c>
+      <c r="EN24" s="8">
+        <f t="shared" si="14"/>
+        <v>3.0507414967512405</v>
+      </c>
+      <c r="EP24" s="9">
         <v>106</v>
       </c>
-      <c r="EM24">
-        <f t="shared" si="11"/>
+      <c r="EQ24" s="8">
+        <f t="shared" si="15"/>
         <v>325.14999999999998</v>
       </c>
-      <c r="EN24">
-        <f t="shared" si="12"/>
+      <c r="ER24" s="8">
+        <f t="shared" si="16"/>
         <v>66.144000000000005</v>
       </c>
-      <c r="EP24" s="2">
+      <c r="ES24" s="8">
+        <f t="shared" si="17"/>
+        <v>91.287485451183443</v>
+      </c>
+      <c r="ET24" s="8">
+        <f t="shared" si="18"/>
+        <v>27.693129978389887</v>
+      </c>
+      <c r="EV24" s="9">
         <f>0.158*100</f>
         <v>15.8</v>
       </c>
-      <c r="EQ24">
-        <f t="shared" si="13"/>
+      <c r="EW24" s="8">
+        <f t="shared" si="19"/>
         <v>28.681999999999999</v>
       </c>
-      <c r="ER24">
-        <f t="shared" si="14"/>
+      <c r="EX24" s="8">
+        <f t="shared" si="20"/>
         <v>22.363500000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY24" s="8">
+        <f t="shared" si="21"/>
+        <v>9.216429785985456</v>
+      </c>
+      <c r="EZ24" s="8">
+        <f t="shared" si="22"/>
+        <v>7.0830886271456377</v>
+      </c>
+    </row>
+    <row r="25" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>68.300000000000011</v>
       </c>
@@ -9847,58 +10636,86 @@
       <c r="EB25">
         <v>8.2759999999999998</v>
       </c>
-      <c r="ED25" s="2">
+      <c r="ED25" s="9">
         <v>146</v>
       </c>
-      <c r="EE25">
-        <f t="shared" si="15"/>
+      <c r="EE25" s="8">
+        <f t="shared" si="23"/>
         <v>29.88100725</v>
       </c>
-      <c r="EF25">
+      <c r="EF25" s="8">
         <f t="shared" si="8"/>
         <v>20.304499999999997</v>
       </c>
-      <c r="EH25" s="2">
+      <c r="EG25" s="8">
+        <f t="shared" si="9"/>
+        <v>42.256690990659756</v>
+      </c>
+      <c r="EH25" s="8">
+        <f t="shared" si="10"/>
+        <v>2.0506096654409816E-2</v>
+      </c>
+      <c r="EJ25" s="9">
         <f>0.199*100</f>
         <v>19.900000000000002</v>
       </c>
-      <c r="EI25">
-        <f t="shared" si="9"/>
+      <c r="EK25" s="8">
+        <f t="shared" si="11"/>
         <v>5.5410500000000003</v>
       </c>
-      <c r="EJ25">
-        <f t="shared" si="10"/>
+      <c r="EL25" s="8">
+        <f t="shared" si="12"/>
         <v>6.5019999999999998</v>
       </c>
-      <c r="EL25" s="2">
+      <c r="EM25" s="8">
+        <f t="shared" si="13"/>
+        <v>0.5586850678154911</v>
+      </c>
+      <c r="EN25" s="8">
+        <f t="shared" si="14"/>
+        <v>2.5088148596498701</v>
+      </c>
+      <c r="EP25" s="9">
         <v>146</v>
       </c>
-      <c r="EM25">
-        <f t="shared" si="11"/>
+      <c r="EQ25" s="8">
+        <f t="shared" si="15"/>
         <v>320.81</v>
       </c>
-      <c r="EN25">
-        <f t="shared" si="12"/>
+      <c r="ER25" s="8">
+        <f t="shared" si="16"/>
         <v>49.347999999999999</v>
       </c>
-      <c r="EP25" s="5">
+      <c r="ES25" s="8">
+        <f t="shared" si="17"/>
+        <v>103.49214849446305</v>
+      </c>
+      <c r="ET25" s="8">
+        <f t="shared" si="18"/>
+        <v>27.667674134267255</v>
+      </c>
+      <c r="EV25" s="9">
         <f>0.199*100</f>
         <v>19.900000000000002</v>
       </c>
-      <c r="EQ25" s="6">
-        <f t="shared" si="13"/>
+      <c r="EW25" s="8">
+        <f t="shared" si="19"/>
         <v>17.5745</v>
       </c>
-      <c r="ER25" s="6">
-        <f t="shared" si="14"/>
+      <c r="EX25" s="8">
+        <f t="shared" si="20"/>
         <v>18.109000000000002</v>
       </c>
-      <c r="ES25">
-        <f>AVERAGE(EQ25:ER25)</f>
-        <v>17.841750000000001</v>
-      </c>
-    </row>
-    <row r="26" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY25" s="8">
+        <f t="shared" si="21"/>
+        <v>7.1184439662049765</v>
+      </c>
+      <c r="EZ25" s="8">
+        <f t="shared" si="22"/>
+        <v>7.3482536700905969</v>
+      </c>
+    </row>
+    <row r="26" spans="1:156" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>100</v>
       </c>
@@ -10217,54 +11034,86 @@
       <c r="EB26">
         <v>7.2187999999999999</v>
       </c>
-      <c r="ED26" s="2">
+      <c r="ED26" s="9">
         <v>200</v>
       </c>
-      <c r="EE26">
-        <f t="shared" si="15"/>
+      <c r="EE26" s="8">
+        <f t="shared" si="23"/>
         <v>24.604031899999999</v>
       </c>
-      <c r="EF26">
+      <c r="EF26" s="8">
         <f t="shared" si="8"/>
         <v>74.2</v>
       </c>
-      <c r="EH26" s="2">
+      <c r="EG26" s="8">
+        <f>STDEVA(DO26,DW26)</f>
+        <v>34.789608520965508</v>
+      </c>
+      <c r="EH26" s="8">
+        <f t="shared" si="10"/>
+        <v>10.008389380914391</v>
+      </c>
+      <c r="EJ26" s="9">
         <f>0.251*100</f>
         <v>25.1</v>
       </c>
-      <c r="EI26">
-        <f t="shared" si="9"/>
+      <c r="EK26" s="8">
+        <f t="shared" si="11"/>
         <v>3.9361999999999995</v>
       </c>
-      <c r="EJ26">
-        <f t="shared" si="10"/>
+      <c r="EL26" s="8">
+        <f t="shared" si="12"/>
         <v>5.7400500000000001</v>
       </c>
-      <c r="EL26" s="2">
+      <c r="EM26" s="8">
+        <f t="shared" si="13"/>
+        <v>0.42949665889270877</v>
+      </c>
+      <c r="EN26" s="8">
+        <f t="shared" si="14"/>
+        <v>2.0912683053592134</v>
+      </c>
+      <c r="EP26" s="9">
         <v>200</v>
       </c>
-      <c r="EM26">
-        <f t="shared" si="11"/>
+      <c r="EQ26" s="8">
+        <f t="shared" si="15"/>
         <v>302.685</v>
       </c>
-      <c r="EN26">
-        <f t="shared" si="12"/>
+      <c r="ER26" s="8">
+        <f t="shared" si="16"/>
         <v>20.787500000000001</v>
       </c>
-      <c r="EP26" s="2">
+      <c r="ES26" s="8">
+        <f t="shared" si="17"/>
+        <v>126.25391578085791</v>
+      </c>
+      <c r="ET26" s="8">
+        <f t="shared" si="18"/>
+        <v>14.742469280958328</v>
+      </c>
+      <c r="EV26" s="9">
         <f>0.251*100</f>
         <v>25.1</v>
       </c>
-      <c r="EQ26">
-        <f t="shared" si="13"/>
+      <c r="EW26" s="8">
+        <f t="shared" si="19"/>
         <v>10.793849999999999</v>
       </c>
-      <c r="ER26">
-        <f t="shared" si="14"/>
+      <c r="EX26" s="8">
+        <f t="shared" si="20"/>
         <v>14.443100000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY26" s="8">
+        <f t="shared" si="21"/>
+        <v>4.3390193413950175</v>
+      </c>
+      <c r="EZ26" s="8">
+        <f t="shared" si="22"/>
+        <v>7.1190096516299217</v>
+      </c>
+    </row>
+    <row r="27" spans="1:156" x14ac:dyDescent="0.35">
       <c r="AC27" s="2">
         <f>0.315*100</f>
         <v>31.5</v>
@@ -10399,32 +11248,48 @@
       <c r="EB27">
         <v>6.1256000000000004</v>
       </c>
-      <c r="EH27" s="2">
+      <c r="EJ27" s="9">
         <f>0.315*100</f>
         <v>31.5</v>
       </c>
-      <c r="EI27">
-        <f t="shared" si="9"/>
+      <c r="EK27" s="8">
+        <f t="shared" si="11"/>
         <v>2.7244999999999999</v>
       </c>
-      <c r="EJ27">
-        <f t="shared" si="10"/>
+      <c r="EL27" s="8">
+        <f t="shared" si="12"/>
         <v>4.9251500000000004</v>
       </c>
-      <c r="EP27" s="2">
+      <c r="EM27" s="8">
+        <f t="shared" si="13"/>
+        <v>0.35298770516832456</v>
+      </c>
+      <c r="EN27" s="8">
+        <f t="shared" si="14"/>
+        <v>1.697692670950782</v>
+      </c>
+      <c r="EV27" s="9">
         <f>0.315*100</f>
         <v>31.5</v>
       </c>
-      <c r="EQ27">
-        <f t="shared" si="13"/>
+      <c r="EW27" s="8">
+        <f t="shared" si="19"/>
         <v>6.5563000000000002</v>
       </c>
-      <c r="ER27">
-        <f t="shared" si="14"/>
+      <c r="EX27" s="8">
+        <f t="shared" si="20"/>
         <v>11.4598</v>
       </c>
-    </row>
-    <row r="28" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY27" s="8">
+        <f t="shared" si="21"/>
+        <v>2.3166232365233648</v>
+      </c>
+      <c r="EZ27" s="8">
+        <f t="shared" si="22"/>
+        <v>6.5424347822504085</v>
+      </c>
+    </row>
+    <row r="28" spans="1:156" x14ac:dyDescent="0.35">
       <c r="AC28" s="2">
         <f>0.396*100</f>
         <v>39.6</v>
@@ -10563,32 +11428,48 @@
       <c r="EB28">
         <v>5.0997000000000003</v>
       </c>
-      <c r="EH28" s="2">
+      <c r="EJ28" s="9">
         <f>0.397*100</f>
         <v>39.700000000000003</v>
       </c>
-      <c r="EI28">
-        <f t="shared" si="9"/>
+      <c r="EK28" s="8">
+        <f t="shared" si="11"/>
         <v>1.8887999999999998</v>
       </c>
-      <c r="EJ28">
-        <f t="shared" si="10"/>
+      <c r="EL28" s="8">
+        <f t="shared" si="12"/>
         <v>4.1179500000000004</v>
       </c>
-      <c r="EP28" s="2">
+      <c r="EM28" s="8">
+        <f t="shared" si="13"/>
+        <v>0.34322963158795128</v>
+      </c>
+      <c r="EN28" s="8">
+        <f t="shared" si="14"/>
+        <v>1.3884041648597867</v>
+      </c>
+      <c r="EV28" s="9">
         <f>0.397*100</f>
         <v>39.700000000000003</v>
       </c>
-      <c r="EQ28">
-        <f t="shared" si="13"/>
+      <c r="EW28" s="8">
+        <f t="shared" si="19"/>
         <v>4.0372000000000003</v>
       </c>
-      <c r="ER28">
-        <f t="shared" si="14"/>
+      <c r="EX28" s="8">
+        <f t="shared" si="20"/>
         <v>9.0224499999999992</v>
       </c>
-    </row>
-    <row r="29" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY28" s="8">
+        <f t="shared" si="21"/>
+        <v>1.3922932521563112</v>
+      </c>
+      <c r="EZ28" s="8">
+        <f t="shared" si="22"/>
+        <v>5.5727792532092995</v>
+      </c>
+    </row>
+    <row r="29" spans="1:156" x14ac:dyDescent="0.35">
       <c r="AC29" s="2">
         <f>0.498*100</f>
         <v>49.8</v>
@@ -10723,32 +11604,48 @@
       <c r="EB29">
         <v>4.2107999999999999</v>
       </c>
-      <c r="EH29" s="2">
+      <c r="EJ29" s="9">
         <f>0.499*100</f>
         <v>49.9</v>
       </c>
-      <c r="EI29">
-        <f t="shared" si="9"/>
+      <c r="EK29" s="8">
+        <f t="shared" si="11"/>
         <v>1.2787999999999999</v>
       </c>
-      <c r="EJ29">
-        <f t="shared" si="10"/>
+      <c r="EL29" s="8">
+        <f t="shared" si="12"/>
         <v>3.3932000000000002</v>
       </c>
-      <c r="EP29" s="2">
+      <c r="EM29" s="8">
+        <f t="shared" si="13"/>
+        <v>0.26827631278217601</v>
+      </c>
+      <c r="EN29" s="8">
+        <f t="shared" si="14"/>
+        <v>1.1562610085962415</v>
+      </c>
+      <c r="EV29" s="9">
         <f>0.499*100</f>
         <v>49.9</v>
       </c>
-      <c r="EQ29">
-        <f t="shared" si="13"/>
+      <c r="EW29" s="8">
+        <f t="shared" si="19"/>
         <v>2.3048500000000001</v>
       </c>
-      <c r="ER29">
-        <f t="shared" si="14"/>
+      <c r="EX29" s="8">
+        <f t="shared" si="20"/>
         <v>6.9077999999999999</v>
       </c>
-    </row>
-    <row r="30" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY29" s="8">
+        <f t="shared" si="21"/>
+        <v>0.87759022613062299</v>
+      </c>
+      <c r="EZ29" s="8">
+        <f t="shared" si="22"/>
+        <v>4.4295997200650064</v>
+      </c>
+    </row>
+    <row r="30" spans="1:156" x14ac:dyDescent="0.35">
       <c r="AC30" s="2">
         <f>0.627*100</f>
         <v>62.7</v>
@@ -10883,32 +11780,48 @@
       <c r="EB30">
         <v>3.3799000000000001</v>
       </c>
-      <c r="EH30" s="2">
+      <c r="EJ30" s="9">
         <f>0.628*100</f>
         <v>62.8</v>
       </c>
-      <c r="EI30">
-        <f t="shared" si="9"/>
+      <c r="EK30" s="8">
+        <f t="shared" si="11"/>
         <v>0.85963499999999993</v>
       </c>
-      <c r="EJ30">
-        <f t="shared" si="10"/>
+      <c r="EL30" s="8">
+        <f t="shared" si="12"/>
         <v>2.7141000000000002</v>
       </c>
-      <c r="EP30" s="2">
+      <c r="EM30" s="8">
+        <f t="shared" si="13"/>
+        <v>0.19751613718883881</v>
+      </c>
+      <c r="EN30" s="8">
+        <f t="shared" si="14"/>
+        <v>0.94158338982800538</v>
+      </c>
+      <c r="EV30" s="9">
         <f>0.628*100</f>
         <v>62.8</v>
       </c>
-      <c r="EQ30">
-        <f t="shared" si="13"/>
+      <c r="EW30" s="8">
+        <f t="shared" si="19"/>
         <v>1.2352300000000001</v>
       </c>
-      <c r="ER30">
-        <f t="shared" si="14"/>
+      <c r="EX30" s="8">
+        <f t="shared" si="20"/>
         <v>5.1089000000000002</v>
       </c>
-    </row>
-    <row r="31" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY30" s="8">
+        <f t="shared" si="21"/>
+        <v>0.61980737798125607</v>
+      </c>
+      <c r="EZ30" s="8">
+        <f t="shared" si="22"/>
+        <v>3.1835361502580737</v>
+      </c>
+    </row>
+    <row r="31" spans="1:156" x14ac:dyDescent="0.35">
       <c r="AC31" s="2">
         <f>0.79*100</f>
         <v>79</v>
@@ -11043,32 +11956,48 @@
       <c r="EB31">
         <v>2.7513000000000001</v>
       </c>
-      <c r="EH31" s="2">
+      <c r="EJ31" s="9">
         <f>0.79*100</f>
         <v>79</v>
       </c>
-      <c r="EI31">
-        <f t="shared" si="9"/>
+      <c r="EK31" s="8">
+        <f t="shared" si="11"/>
         <v>0.57674000000000003</v>
       </c>
-      <c r="EJ31">
-        <f t="shared" si="10"/>
+      <c r="EL31" s="8">
+        <f t="shared" si="12"/>
         <v>2.1869499999999999</v>
       </c>
-      <c r="EP31" s="2">
+      <c r="EM31" s="8">
+        <f t="shared" si="13"/>
+        <v>0.15379572490807425</v>
+      </c>
+      <c r="EN31" s="8">
+        <f t="shared" si="14"/>
+        <v>0.79811142392525691</v>
+      </c>
+      <c r="EV31" s="9">
         <f>0.79*100</f>
         <v>79</v>
       </c>
-      <c r="EQ31">
-        <f t="shared" si="13"/>
+      <c r="EW31" s="8">
+        <f t="shared" si="19"/>
         <v>0.63840000000000008</v>
       </c>
-      <c r="ER31">
-        <f t="shared" si="14"/>
+      <c r="EX31" s="8">
+        <f t="shared" si="20"/>
         <v>3.6128999999999998</v>
       </c>
-    </row>
-    <row r="32" spans="1:149" x14ac:dyDescent="0.35">
+      <c r="EY31" s="8">
+        <f t="shared" si="21"/>
+        <v>0.52184480451567206</v>
+      </c>
+      <c r="EZ31" s="8">
+        <f t="shared" si="22"/>
+        <v>2.0807324143195349</v>
+      </c>
+    </row>
+    <row r="32" spans="1:156" x14ac:dyDescent="0.35">
       <c r="AC32" s="2">
         <f>0.994*100</f>
         <v>99.4</v>
@@ -11203,29 +12132,45 @@
       <c r="EB32">
         <v>2.2105000000000001</v>
       </c>
-      <c r="EH32" s="2">
+      <c r="EJ32" s="9">
         <f>0.995*100</f>
         <v>99.5</v>
       </c>
-      <c r="EI32">
-        <f t="shared" si="9"/>
+      <c r="EK32" s="8">
+        <f t="shared" si="11"/>
         <v>0.37846999999999997</v>
       </c>
-      <c r="EJ32">
-        <f t="shared" si="10"/>
+      <c r="EL32" s="8">
+        <f t="shared" si="12"/>
         <v>1.7681500000000001</v>
       </c>
-      <c r="EP32" s="2">
+      <c r="EM32" s="8">
+        <f t="shared" si="13"/>
+        <v>9.9504066248570999E-2</v>
+      </c>
+      <c r="EN32" s="8">
+        <f t="shared" si="14"/>
+        <v>0.62557736931573849</v>
+      </c>
+      <c r="EV32" s="9">
         <f>0.995*100</f>
         <v>99.5</v>
       </c>
-      <c r="EQ32">
-        <f t="shared" si="13"/>
+      <c r="EW32" s="8">
+        <f t="shared" si="19"/>
         <v>0.33570439999999996</v>
       </c>
-      <c r="ER32">
-        <f t="shared" si="14"/>
+      <c r="EX32" s="8">
+        <f t="shared" si="20"/>
         <v>2.5263499999999999</v>
+      </c>
+      <c r="EY32" s="8">
+        <f t="shared" si="21"/>
+        <v>0.47140772634177314</v>
+      </c>
+      <c r="EZ32" s="8">
+        <f t="shared" si="22"/>
+        <v>1.1766963945725339</v>
       </c>
     </row>
     <row r="141" spans="5:8" x14ac:dyDescent="0.35">

</xml_diff>